<commit_message>
Fixed old workflows and finished FTN007, FTN008 and FTN009
</commit_message>
<xml_diff>
--- a/src/test/resources/data/dataUserArchive.xlsx
+++ b/src/test/resources/data/dataUserArchive.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>MWEyUzNkNEZ0ZXN0UGFzc3dvcmQ=</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>dXN1YXJpb0ZhbGxpZG8=</t>
+  </si>
+  <si>
+    <t>MTIzNA==</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -420,6 +426,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>